<commit_message>
Add wrangler config for Cloudflare deployment
</commit_message>
<xml_diff>
--- a/mr_market_tracker.xlsx
+++ b/mr_market_tracker.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Static" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Positions" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Action_Log" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Pending_Orders" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Target_History" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Benchmark" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Lessons_Log" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Static" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Positions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Action_Log" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pending_Orders" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Target_History" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Benchmark" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Lessons_Log" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2767,7 +2767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2927,7 +2927,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>179.97</v>
+        <v>280</v>
       </c>
       <c r="D4" t="n">
         <v>12</v>
@@ -3033,211 +3033,6 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2026-01-14</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>310.18</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Target Hit</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Intact</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>GTC from broker</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2026-01-09</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PWR</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>350.35</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Target Hit</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Intact</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>GTC from broker</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2026-01-08</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CB</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>179.97</v>
-      </c>
-      <c r="D9" t="n">
-        <v>12</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Target Hit</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Intact</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>GTC from broker</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2026-01-08</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>CVX</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>149.47</v>
-      </c>
-      <c r="D10" t="n">
-        <v>15</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Target Hit</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Intact</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>GTC from broker</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2026-01-08</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>CPRT</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>34.97</v>
-      </c>
-      <c r="D11" t="n">
-        <v>60</v>
-      </c>
-      <c r="E11" t="n">
-        <v>3</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Target Hit</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Intact</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>GTC from broker</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
         <is>
           <t>PENDING</t>
         </is>
@@ -3307,7 +3102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3446,6 +3241,50 @@
         <v>0.1219050064086914</v>
       </c>
       <c r="F5" s="6" t="n">
+        <v>0.1203328596126897</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>637.0900268554688</v>
+      </c>
+      <c r="C6" t="n">
+        <v>44876.20025634766</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0.001572146796001695</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0.1219050064086914</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0.1203328596126897</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>637.0900268554688</v>
+      </c>
+      <c r="C7" t="n">
+        <v>44876.20025634766</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>0.001572146796001695</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>0.1219050064086914</v>
+      </c>
+      <c r="F7" s="6" t="n">
         <v>0.1203328596126897</v>
       </c>
     </row>

</xml_diff>